<commit_message>
[kbss-cvut/termit-ui#449] Handle null cells in imported Excel.
Null cells occur when there are no more columns after them.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/termit-import.xlsx
+++ b/src/main/resources/template/termit-import.xlsx
@@ -130,10 +130,10 @@
 - To add translations in another language, copy the "English" sheet and label it using the name of the language the sheet will represent</t>
   </si>
   <si>
-    <t xml:space="preserve">- Rodičovské pojmy musí být deklarovány před svými potomky</t>
+    <t xml:space="preserve">- Pro jiné jazyky než češtinu a angličtinu použijte anglické názvy sloupců</t>
   </si>
   <si>
-    <t xml:space="preserve">- Parent terms must be declared before their children</t>
+    <t xml:space="preserve">- Use English column labels for sheets in languages other than Czech and English</t>
   </si>
 </sst>
 </file>
@@ -272,10 +272,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.25"/>
@@ -17345,7 +17345,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
@@ -34412,10 +34412,10 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="75.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>

</xml_diff>

<commit_message>
[kbss-cvut/termit-ui#449] Use semicolon when splitting multiple values in imported Excel cell.
Semicolon is used in export as well.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/termit-import.xlsx
+++ b/src/main/resources/template/termit-import.xlsx
@@ -120,12 +120,12 @@
     <t xml:space="preserve">Manual</t>
   </si>
   <si>
-    <t xml:space="preserve">- Pro vícehodnotové položky použijte jako oddělovač čárku (,)
+    <t xml:space="preserve">- Pro vícehodnotové položky použijte jako oddělovač středník (;)
 - Pro referencování jiných pojmů použijte jejich název (např. související pojmy, pojmy se stejným významem)
 - Pro přidání dalšího jazyka zkopírujte sheet "English" a pojmenujte ho názvem jazyku, který daný sheet reprezentuje</t>
   </si>
   <si>
-    <t xml:space="preserve">- Use comma (,) to separate values in multi-valued attributes
+    <t xml:space="preserve">- Use a semicolon (;) to separate values in multi-valued attributes
 - Use labels of terms you want to reference (e.g., related terms, exact matches)
 - To add translations in another language, copy the "English" sheet and label it using the name of the language the sheet will represent</t>
   </si>
@@ -272,7 +272,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
@@ -17345,7 +17345,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
@@ -34412,10 +34412,10 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="75.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
@@ -34430,7 +34430,7 @@
       </c>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
[kbss-cvut/termit-ui#449] Use first state and type encountered for a term.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/termit-import.xlsx
+++ b/src/main/resources/template/termit-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Czech" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Název</t>
   </si>
@@ -103,12 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">- Pro vícehodnotové položky použijte jako oddělovač středník (;)
-- Pro referencování jiných pojmů použijte jejich název (např. související pojmy, pojmy se stejným významem)
+- Pro referencování jiných pojmů použijte jejich název (např. Nadřazené pojmy, související pojmy)
 - Pro přidání dalšího jazyka zkopírujte sheet "English" a pojmenujte ho názvem jazyku, který daný sheet reprezentuje</t>
   </si>
   <si>
     <t xml:space="preserve">- Use a semicolon (;) to separate values in multi-valued attributes
-- Use labels of terms you want to reference (e.g., related terms, exact matches)
+- Use labels of terms you want to reference (e.g., broader terms, related terms)
 - To add translations in another language, copy the "English" sheet and label it using the name of the language the sheet will represent</t>
   </si>
   <si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t xml:space="preserve">- Use English column labels for sheets in languages other than Czech and English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Import použije první dostupný stav a typ. Pokud se tedy v různých sheetech vyskytují různé hodnoty stavu a typu, jsou použity první z ních.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- The import with use the first available value of state and type. Thus if multiple sheets contain different values of state and type, the first ones are used.</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,8 +225,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -254,7 +268,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.27"/>
@@ -15318,11 +15332,11 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
@@ -28371,48 +28385,55 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="75.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="75.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="75.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="4"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>